<commit_message>
Rough draft of text
Rough draft of text and updated sample numbers to reach 500.
</commit_message>
<xml_diff>
--- a/data/metaB_effort.xlsx
+++ b/data/metaB_effort.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jacob_cochran_fws_gov/Documents/Early Detection Monitoring/Implementation_Planning/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/colleen_keefer_fws_gov/Documents/Desktop/Automation tool github/Implementation_Planning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{544D56E2-6810-4C87-AC3D-3B7FD940DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2E2DA6C-723E-4156-AA0A-B056C5FD6549}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{544D56E2-6810-4C87-AC3D-3B7FD940DA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB76DA9-E943-4AE9-872A-200D5C95EC43}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{E30D9601-8F6E-4B6E-AA75-88F8C03488F9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{E30D9601-8F6E-4B6E-AA75-88F8C03488F9}"/>
   </bookViews>
   <sheets>
     <sheet name="metaB_effort" sheetId="1" r:id="rId1"/>
@@ -1013,25 +1013,25 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.41796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1671,13 +1671,13 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1703,13 +1703,13 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>33</v>
       </c>

</xml_diff>